<commit_message>
refactoring code : integrate excel file when has data
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/file1.xlsx
+++ b/src/test/resources/excel/file1.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="480" yWindow="60" windowWidth="22038" windowHeight="9654"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="f1-s1" sheetId="1" r:id="rId1"/>
+    <sheet name="f1-s2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -404,12 +404,55 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>800</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>